<commit_message>
Erhöhung auf 1h Raus aus Testphase Ver. 1.1
</commit_message>
<xml_diff>
--- a/station_data_analysis.xlsx
+++ b/station_data_analysis.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D44"/>
+  <dimension ref="A2:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,11 +464,11 @@
         <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>1709639415</v>
+        <v>1709640348</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2024-03-05 12:52:54.415934</t>
+          <t>2024-03-05 13:28:02.412210</t>
         </is>
       </c>
     </row>
@@ -482,11 +482,11 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>1709639415</v>
+        <v>1709640348</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2024-03-05 12:52:54.415934</t>
+          <t>2024-03-05 13:28:02.412210</t>
         </is>
       </c>
     </row>
@@ -500,11 +500,11 @@
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>1709639415</v>
+        <v>1709640349</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2024-03-05 12:52:54.415934</t>
+          <t>2024-03-05 13:28:02.412210</t>
         </is>
       </c>
     </row>
@@ -518,11 +518,11 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>1709639415</v>
+        <v>1709640349</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2024-03-05 12:52:54.415934</t>
+          <t>2024-03-05 13:28:02.412210</t>
         </is>
       </c>
     </row>
@@ -536,11 +536,11 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>1709639415</v>
+        <v>1709640349</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2024-03-05 12:52:54.415934</t>
+          <t>2024-03-05 13:28:02.412210</t>
         </is>
       </c>
     </row>
@@ -554,11 +554,11 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>1709639415</v>
+        <v>1709640349</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2024-03-05 12:52:54.415934</t>
+          <t>2024-03-05 13:28:02.412210</t>
         </is>
       </c>
     </row>
@@ -572,11 +572,11 @@
         <v>2</v>
       </c>
       <c r="C9" t="n">
-        <v>1709639415</v>
+        <v>1709640349</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2024-03-05 12:52:54.415934</t>
+          <t>2024-03-05 13:28:02.412210</t>
         </is>
       </c>
     </row>
@@ -590,11 +590,11 @@
         <v>2</v>
       </c>
       <c r="C10" t="n">
-        <v>1709639415</v>
+        <v>1709640349</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2024-03-05 12:52:54.415934</t>
+          <t>2024-03-05 13:28:02.412210</t>
         </is>
       </c>
     </row>
@@ -608,11 +608,11 @@
         <v>2</v>
       </c>
       <c r="C11" t="n">
-        <v>1709639416</v>
+        <v>1709640349</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2024-03-05 12:52:54.415934</t>
+          <t>2024-03-05 13:28:02.412210</t>
         </is>
       </c>
     </row>
@@ -626,11 +626,11 @@
         <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>1709639416</v>
+        <v>1709640349</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2024-03-05 12:52:54.415934</t>
+          <t>2024-03-05 13:28:02.412210</t>
         </is>
       </c>
     </row>
@@ -644,11 +644,11 @@
         <v>8</v>
       </c>
       <c r="C13" t="n">
-        <v>1709639416</v>
+        <v>1709640349</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2024-03-05 12:52:54.415934</t>
+          <t>2024-03-05 13:28:02.412210</t>
         </is>
       </c>
     </row>
@@ -662,11 +662,11 @@
         <v>2</v>
       </c>
       <c r="C14" t="n">
-        <v>1709639416</v>
+        <v>1709640349</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2024-03-05 12:52:54.415934</t>
+          <t>2024-03-05 13:28:02.412210</t>
         </is>
       </c>
     </row>
@@ -680,11 +680,11 @@
         <v>2</v>
       </c>
       <c r="C15" t="n">
-        <v>1709639416</v>
+        <v>1709640349</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2024-03-05 12:52:54.415934</t>
+          <t>2024-03-05 13:28:02.412210</t>
         </is>
       </c>
     </row>
@@ -698,515 +698,11 @@
         <v>2</v>
       </c>
       <c r="C16" t="n">
-        <v>1709639416</v>
+        <v>1709640349</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2024-03-05 12:52:54.415934</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>CAB:Station:958219cd-8009-45b6-8a04-1cc4ae763307</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>5</v>
-      </c>
-      <c r="C17" t="n">
-        <v>1709640348</v>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>2024-03-05 13:07:54.939505</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>CAB:Station:69a20737-5c07-4ab4-ad8a-4fcba602ef6b</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>3</v>
-      </c>
-      <c r="C18" t="n">
-        <v>1709640348</v>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>2024-03-05 13:07:54.939505</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>CAB:Station:59830a25-c7c6-4c9b-af21-0b67c836ba8f</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>6</v>
-      </c>
-      <c r="C19" t="n">
-        <v>1709640349</v>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>2024-03-05 13:07:54.939505</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>CAB:Station:36fe6a30-d53e-4aa8-863d-e21e80fd1d0b</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>5</v>
-      </c>
-      <c r="C20" t="n">
-        <v>1709640349</v>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>2024-03-05 13:07:54.939505</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>CAB:Station:ca41b63e-9046-442f-880e-d0e9186e507a</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>0</v>
-      </c>
-      <c r="C21" t="n">
-        <v>1709640349</v>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>2024-03-05 13:07:54.939505</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>CAB:Station:714932fd-4836-4a2a-9a19-07a6d694274c</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>7</v>
-      </c>
-      <c r="C22" t="n">
-        <v>1709640349</v>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>2024-03-05 13:07:54.939505</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>CAB:Station:7046d131-47fd-40bd-ba63-f52590d2ee8f</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>2</v>
-      </c>
-      <c r="C23" t="n">
-        <v>1709640349</v>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>2024-03-05 13:07:54.939505</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>CAB:Station:e375c577-ca9b-4f3d-b052-582f4eeeb0a8</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>2</v>
-      </c>
-      <c r="C24" t="n">
-        <v>1709640349</v>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>2024-03-05 13:07:54.939505</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>CAB:Station:f384359e-349d-47cf-aec3-031f20b8e0a0</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>2</v>
-      </c>
-      <c r="C25" t="n">
-        <v>1709640349</v>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>2024-03-05 13:07:54.939505</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>CAB:Station:e73ff873-8f43-41b4-868a-2d3e00f2cfbb</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>2</v>
-      </c>
-      <c r="C26" t="n">
-        <v>1709640349</v>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>2024-03-05 13:07:54.939505</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>CAB:Station:c070e40c-98f6-45d6-9543-90ceceef63af</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>8</v>
-      </c>
-      <c r="C27" t="n">
-        <v>1709640349</v>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>2024-03-05 13:07:54.939505</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>CAB:Station:2263b695-db35-4bbf-b70a-032920fadf3f</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>2</v>
-      </c>
-      <c r="C28" t="n">
-        <v>1709640349</v>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>2024-03-05 13:07:54.939505</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>CAB:Station:be796eb3-49af-494c-b3f0-dc1f0132eb7d</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>2</v>
-      </c>
-      <c r="C29" t="n">
-        <v>1709640349</v>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>2024-03-05 13:07:54.939505</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>CAB:Station:b207ab7a-f23d-40f8-aa26-5d02077fc6f9</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
-        <v>2</v>
-      </c>
-      <c r="C30" t="n">
-        <v>1709640349</v>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>2024-03-05 13:07:54.939505</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>CAB:Station:958219cd-8009-45b6-8a04-1cc4ae763307</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>5</v>
-      </c>
-      <c r="C31" t="n">
-        <v>1709640348</v>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>2024-03-05 13:22:55.422522</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>CAB:Station:69a20737-5c07-4ab4-ad8a-4fcba602ef6b</t>
-        </is>
-      </c>
-      <c r="B32" t="n">
-        <v>3</v>
-      </c>
-      <c r="C32" t="n">
-        <v>1709640348</v>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>2024-03-05 13:22:55.422522</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>CAB:Station:59830a25-c7c6-4c9b-af21-0b67c836ba8f</t>
-        </is>
-      </c>
-      <c r="B33" t="n">
-        <v>6</v>
-      </c>
-      <c r="C33" t="n">
-        <v>1709640349</v>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>2024-03-05 13:22:55.422522</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>CAB:Station:36fe6a30-d53e-4aa8-863d-e21e80fd1d0b</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>5</v>
-      </c>
-      <c r="C34" t="n">
-        <v>1709640349</v>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>2024-03-05 13:22:55.422522</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>CAB:Station:ca41b63e-9046-442f-880e-d0e9186e507a</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>0</v>
-      </c>
-      <c r="C35" t="n">
-        <v>1709640349</v>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>2024-03-05 13:22:55.422522</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>CAB:Station:714932fd-4836-4a2a-9a19-07a6d694274c</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>7</v>
-      </c>
-      <c r="C36" t="n">
-        <v>1709640349</v>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>2024-03-05 13:22:55.422522</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>CAB:Station:7046d131-47fd-40bd-ba63-f52590d2ee8f</t>
-        </is>
-      </c>
-      <c r="B37" t="n">
-        <v>2</v>
-      </c>
-      <c r="C37" t="n">
-        <v>1709640349</v>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>2024-03-05 13:22:55.422522</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>CAB:Station:e375c577-ca9b-4f3d-b052-582f4eeeb0a8</t>
-        </is>
-      </c>
-      <c r="B38" t="n">
-        <v>2</v>
-      </c>
-      <c r="C38" t="n">
-        <v>1709640349</v>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>2024-03-05 13:22:55.422522</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>CAB:Station:f384359e-349d-47cf-aec3-031f20b8e0a0</t>
-        </is>
-      </c>
-      <c r="B39" t="n">
-        <v>2</v>
-      </c>
-      <c r="C39" t="n">
-        <v>1709640349</v>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>2024-03-05 13:22:55.422522</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>CAB:Station:e73ff873-8f43-41b4-868a-2d3e00f2cfbb</t>
-        </is>
-      </c>
-      <c r="B40" t="n">
-        <v>2</v>
-      </c>
-      <c r="C40" t="n">
-        <v>1709640349</v>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>2024-03-05 13:22:55.422522</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>CAB:Station:c070e40c-98f6-45d6-9543-90ceceef63af</t>
-        </is>
-      </c>
-      <c r="B41" t="n">
-        <v>8</v>
-      </c>
-      <c r="C41" t="n">
-        <v>1709640349</v>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>2024-03-05 13:22:55.422522</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>CAB:Station:2263b695-db35-4bbf-b70a-032920fadf3f</t>
-        </is>
-      </c>
-      <c r="B42" t="n">
-        <v>2</v>
-      </c>
-      <c r="C42" t="n">
-        <v>1709640349</v>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>2024-03-05 13:22:55.422522</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>CAB:Station:be796eb3-49af-494c-b3f0-dc1f0132eb7d</t>
-        </is>
-      </c>
-      <c r="B43" t="n">
-        <v>2</v>
-      </c>
-      <c r="C43" t="n">
-        <v>1709640349</v>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>2024-03-05 13:22:55.422522</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>CAB:Station:b207ab7a-f23d-40f8-aa26-5d02077fc6f9</t>
-        </is>
-      </c>
-      <c r="B44" t="n">
-        <v>2</v>
-      </c>
-      <c r="C44" t="n">
-        <v>1709640349</v>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>2024-03-05 13:22:55.422522</t>
+          <t>2024-03-05 13:28:02.412210</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auswertung fertig Version 1.0 Excel Pull 3
</commit_message>
<xml_diff>
--- a/station_data_analysis.xlsx
+++ b/station_data_analysis.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D58"/>
+  <dimension ref="A2:D72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1462,6 +1462,258 @@
         </is>
       </c>
     </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>CAB:Station:958219cd-8009-45b6-8a04-1cc4ae763307</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>5</v>
+      </c>
+      <c r="C59" t="n">
+        <v>1709651610</v>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>2024-03-05 16:16:16.319954</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>CAB:Station:69a20737-5c07-4ab4-ad8a-4fcba602ef6b</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>3</v>
+      </c>
+      <c r="C60" t="n">
+        <v>1709651610</v>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>2024-03-05 16:16:16.319954</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>CAB:Station:59830a25-c7c6-4c9b-af21-0b67c836ba8f</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>5</v>
+      </c>
+      <c r="C61" t="n">
+        <v>1709651610</v>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>2024-03-05 16:16:16.319954</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>CAB:Station:36fe6a30-d53e-4aa8-863d-e21e80fd1d0b</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>5</v>
+      </c>
+      <c r="C62" t="n">
+        <v>1709651610</v>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>2024-03-05 16:16:16.319954</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>CAB:Station:ca41b63e-9046-442f-880e-d0e9186e507a</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>1</v>
+      </c>
+      <c r="C63" t="n">
+        <v>1709651610</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>2024-03-05 16:16:16.319954</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>CAB:Station:714932fd-4836-4a2a-9a19-07a6d694274c</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>7</v>
+      </c>
+      <c r="C64" t="n">
+        <v>1709651610</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>2024-03-05 16:16:16.319954</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>CAB:Station:7046d131-47fd-40bd-ba63-f52590d2ee8f</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>2</v>
+      </c>
+      <c r="C65" t="n">
+        <v>1709651610</v>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>2024-03-05 16:16:16.319954</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>CAB:Station:e375c577-ca9b-4f3d-b052-582f4eeeb0a8</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>2</v>
+      </c>
+      <c r="C66" t="n">
+        <v>1709651610</v>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>2024-03-05 16:16:16.319954</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>CAB:Station:f384359e-349d-47cf-aec3-031f20b8e0a0</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>2</v>
+      </c>
+      <c r="C67" t="n">
+        <v>1709651610</v>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>2024-03-05 16:16:16.319954</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>CAB:Station:e73ff873-8f43-41b4-868a-2d3e00f2cfbb</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>2</v>
+      </c>
+      <c r="C68" t="n">
+        <v>1709651610</v>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>2024-03-05 16:16:16.319954</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>CAB:Station:c070e40c-98f6-45d6-9543-90ceceef63af</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>9</v>
+      </c>
+      <c r="C69" t="n">
+        <v>1709651610</v>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>2024-03-05 16:16:16.319954</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>CAB:Station:2263b695-db35-4bbf-b70a-032920fadf3f</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>1</v>
+      </c>
+      <c r="C70" t="n">
+        <v>1709651610</v>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>2024-03-05 16:16:16.319954</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>CAB:Station:be796eb3-49af-494c-b3f0-dc1f0132eb7d</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>2</v>
+      </c>
+      <c r="C71" t="n">
+        <v>1709651610</v>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>2024-03-05 16:16:16.319954</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>CAB:Station:b207ab7a-f23d-40f8-aa26-5d02077fc6f9</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>2</v>
+      </c>
+      <c r="C72" t="n">
+        <v>1709651610</v>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>2024-03-05 16:16:16.319954</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finish mit einfachem filter
</commit_message>
<xml_diff>
--- a/station_data_analysis.xlsx
+++ b/station_data_analysis.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D128"/>
+  <dimension ref="A2:D296"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2722,6 +2722,3030 @@
         </is>
       </c>
     </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>CAB:Station:958219cd-8009-45b6-8a04-1cc4ae763307</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
+        <v>5</v>
+      </c>
+      <c r="C129" t="n">
+        <v>1709838832</v>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>2024-03-08 07:41:01.401853</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>CAB:Station:69a20737-5c07-4ab4-ad8a-4fcba602ef6b</t>
+        </is>
+      </c>
+      <c r="B130" t="n">
+        <v>3</v>
+      </c>
+      <c r="C130" t="n">
+        <v>1709838832</v>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>2024-03-08 07:41:01.401853</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>CAB:Station:59830a25-c7c6-4c9b-af21-0b67c836ba8f</t>
+        </is>
+      </c>
+      <c r="B131" t="n">
+        <v>5</v>
+      </c>
+      <c r="C131" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>2024-03-08 07:41:01.401853</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>CAB:Station:36fe6a30-d53e-4aa8-863d-e21e80fd1d0b</t>
+        </is>
+      </c>
+      <c r="B132" t="n">
+        <v>5</v>
+      </c>
+      <c r="C132" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>2024-03-08 07:41:01.401853</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>CAB:Station:ca41b63e-9046-442f-880e-d0e9186e507a</t>
+        </is>
+      </c>
+      <c r="B133" t="n">
+        <v>4</v>
+      </c>
+      <c r="C133" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>2024-03-08 07:41:01.401853</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>CAB:Station:714932fd-4836-4a2a-9a19-07a6d694274c</t>
+        </is>
+      </c>
+      <c r="B134" t="n">
+        <v>2</v>
+      </c>
+      <c r="C134" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>2024-03-08 07:41:01.401853</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>CAB:Station:7046d131-47fd-40bd-ba63-f52590d2ee8f</t>
+        </is>
+      </c>
+      <c r="B135" t="n">
+        <v>2</v>
+      </c>
+      <c r="C135" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>2024-03-08 07:41:01.401853</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>CAB:Station:e375c577-ca9b-4f3d-b052-582f4eeeb0a8</t>
+        </is>
+      </c>
+      <c r="B136" t="n">
+        <v>3</v>
+      </c>
+      <c r="C136" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>2024-03-08 07:41:01.401853</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>CAB:Station:f384359e-349d-47cf-aec3-031f20b8e0a0</t>
+        </is>
+      </c>
+      <c r="B137" t="n">
+        <v>2</v>
+      </c>
+      <c r="C137" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>2024-03-08 07:41:01.401853</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>CAB:Station:e73ff873-8f43-41b4-868a-2d3e00f2cfbb</t>
+        </is>
+      </c>
+      <c r="B138" t="n">
+        <v>3</v>
+      </c>
+      <c r="C138" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>2024-03-08 07:41:01.401853</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>CAB:Station:c070e40c-98f6-45d6-9543-90ceceef63af</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>8</v>
+      </c>
+      <c r="C139" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>2024-03-08 07:41:01.401853</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>CAB:Station:2263b695-db35-4bbf-b70a-032920fadf3f</t>
+        </is>
+      </c>
+      <c r="B140" t="n">
+        <v>0</v>
+      </c>
+      <c r="C140" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>2024-03-08 07:41:01.401853</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>CAB:Station:be796eb3-49af-494c-b3f0-dc1f0132eb7d</t>
+        </is>
+      </c>
+      <c r="B141" t="n">
+        <v>1</v>
+      </c>
+      <c r="C141" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>2024-03-08 07:41:01.401853</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>CAB:Station:b207ab7a-f23d-40f8-aa26-5d02077fc6f9</t>
+        </is>
+      </c>
+      <c r="B142" t="n">
+        <v>1</v>
+      </c>
+      <c r="C142" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>2024-03-08 07:41:01.401853</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>CAB:Station:958219cd-8009-45b6-8a04-1cc4ae763307</t>
+        </is>
+      </c>
+      <c r="B143" t="n">
+        <v>5</v>
+      </c>
+      <c r="C143" t="n">
+        <v>1709838832</v>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>2024-03-08 07:56:01.968412</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>CAB:Station:69a20737-5c07-4ab4-ad8a-4fcba602ef6b</t>
+        </is>
+      </c>
+      <c r="B144" t="n">
+        <v>3</v>
+      </c>
+      <c r="C144" t="n">
+        <v>1709838832</v>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>2024-03-08 07:56:01.968412</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>CAB:Station:59830a25-c7c6-4c9b-af21-0b67c836ba8f</t>
+        </is>
+      </c>
+      <c r="B145" t="n">
+        <v>5</v>
+      </c>
+      <c r="C145" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>2024-03-08 07:56:01.968412</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>CAB:Station:36fe6a30-d53e-4aa8-863d-e21e80fd1d0b</t>
+        </is>
+      </c>
+      <c r="B146" t="n">
+        <v>5</v>
+      </c>
+      <c r="C146" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>2024-03-08 07:56:01.968412</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>CAB:Station:ca41b63e-9046-442f-880e-d0e9186e507a</t>
+        </is>
+      </c>
+      <c r="B147" t="n">
+        <v>4</v>
+      </c>
+      <c r="C147" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>2024-03-08 07:56:01.968412</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>CAB:Station:714932fd-4836-4a2a-9a19-07a6d694274c</t>
+        </is>
+      </c>
+      <c r="B148" t="n">
+        <v>2</v>
+      </c>
+      <c r="C148" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>2024-03-08 07:56:01.968412</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>CAB:Station:7046d131-47fd-40bd-ba63-f52590d2ee8f</t>
+        </is>
+      </c>
+      <c r="B149" t="n">
+        <v>2</v>
+      </c>
+      <c r="C149" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>2024-03-08 07:56:01.968412</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>CAB:Station:e375c577-ca9b-4f3d-b052-582f4eeeb0a8</t>
+        </is>
+      </c>
+      <c r="B150" t="n">
+        <v>3</v>
+      </c>
+      <c r="C150" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>2024-03-08 07:56:01.968412</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>CAB:Station:f384359e-349d-47cf-aec3-031f20b8e0a0</t>
+        </is>
+      </c>
+      <c r="B151" t="n">
+        <v>2</v>
+      </c>
+      <c r="C151" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>2024-03-08 07:56:01.968412</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>CAB:Station:e73ff873-8f43-41b4-868a-2d3e00f2cfbb</t>
+        </is>
+      </c>
+      <c r="B152" t="n">
+        <v>3</v>
+      </c>
+      <c r="C152" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>2024-03-08 07:56:01.968412</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>CAB:Station:c070e40c-98f6-45d6-9543-90ceceef63af</t>
+        </is>
+      </c>
+      <c r="B153" t="n">
+        <v>8</v>
+      </c>
+      <c r="C153" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>2024-03-08 07:56:01.968412</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>CAB:Station:2263b695-db35-4bbf-b70a-032920fadf3f</t>
+        </is>
+      </c>
+      <c r="B154" t="n">
+        <v>0</v>
+      </c>
+      <c r="C154" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>2024-03-08 07:56:01.968412</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>CAB:Station:be796eb3-49af-494c-b3f0-dc1f0132eb7d</t>
+        </is>
+      </c>
+      <c r="B155" t="n">
+        <v>1</v>
+      </c>
+      <c r="C155" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>2024-03-08 07:56:01.968412</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>CAB:Station:b207ab7a-f23d-40f8-aa26-5d02077fc6f9</t>
+        </is>
+      </c>
+      <c r="B156" t="n">
+        <v>1</v>
+      </c>
+      <c r="C156" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>2024-03-08 07:56:01.968412</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>CAB:Station:958219cd-8009-45b6-8a04-1cc4ae763307</t>
+        </is>
+      </c>
+      <c r="B157" t="n">
+        <v>5</v>
+      </c>
+      <c r="C157" t="n">
+        <v>1709838832</v>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:11:02.453630</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>CAB:Station:69a20737-5c07-4ab4-ad8a-4fcba602ef6b</t>
+        </is>
+      </c>
+      <c r="B158" t="n">
+        <v>3</v>
+      </c>
+      <c r="C158" t="n">
+        <v>1709838832</v>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:11:02.453630</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>CAB:Station:59830a25-c7c6-4c9b-af21-0b67c836ba8f</t>
+        </is>
+      </c>
+      <c r="B159" t="n">
+        <v>5</v>
+      </c>
+      <c r="C159" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:11:02.453630</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>CAB:Station:36fe6a30-d53e-4aa8-863d-e21e80fd1d0b</t>
+        </is>
+      </c>
+      <c r="B160" t="n">
+        <v>5</v>
+      </c>
+      <c r="C160" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:11:02.453630</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>CAB:Station:ca41b63e-9046-442f-880e-d0e9186e507a</t>
+        </is>
+      </c>
+      <c r="B161" t="n">
+        <v>4</v>
+      </c>
+      <c r="C161" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:11:02.453630</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>CAB:Station:714932fd-4836-4a2a-9a19-07a6d694274c</t>
+        </is>
+      </c>
+      <c r="B162" t="n">
+        <v>2</v>
+      </c>
+      <c r="C162" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:11:02.453630</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>CAB:Station:7046d131-47fd-40bd-ba63-f52590d2ee8f</t>
+        </is>
+      </c>
+      <c r="B163" t="n">
+        <v>2</v>
+      </c>
+      <c r="C163" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:11:02.453630</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>CAB:Station:e375c577-ca9b-4f3d-b052-582f4eeeb0a8</t>
+        </is>
+      </c>
+      <c r="B164" t="n">
+        <v>3</v>
+      </c>
+      <c r="C164" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:11:02.453630</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>CAB:Station:f384359e-349d-47cf-aec3-031f20b8e0a0</t>
+        </is>
+      </c>
+      <c r="B165" t="n">
+        <v>2</v>
+      </c>
+      <c r="C165" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:11:02.453630</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>CAB:Station:e73ff873-8f43-41b4-868a-2d3e00f2cfbb</t>
+        </is>
+      </c>
+      <c r="B166" t="n">
+        <v>3</v>
+      </c>
+      <c r="C166" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:11:02.453630</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>CAB:Station:c070e40c-98f6-45d6-9543-90ceceef63af</t>
+        </is>
+      </c>
+      <c r="B167" t="n">
+        <v>8</v>
+      </c>
+      <c r="C167" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:11:02.453630</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>CAB:Station:2263b695-db35-4bbf-b70a-032920fadf3f</t>
+        </is>
+      </c>
+      <c r="B168" t="n">
+        <v>0</v>
+      </c>
+      <c r="C168" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:11:02.453630</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>CAB:Station:be796eb3-49af-494c-b3f0-dc1f0132eb7d</t>
+        </is>
+      </c>
+      <c r="B169" t="n">
+        <v>1</v>
+      </c>
+      <c r="C169" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:11:02.453630</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>CAB:Station:b207ab7a-f23d-40f8-aa26-5d02077fc6f9</t>
+        </is>
+      </c>
+      <c r="B170" t="n">
+        <v>1</v>
+      </c>
+      <c r="C170" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:11:02.453630</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>CAB:Station:958219cd-8009-45b6-8a04-1cc4ae763307</t>
+        </is>
+      </c>
+      <c r="B171" t="n">
+        <v>5</v>
+      </c>
+      <c r="C171" t="n">
+        <v>1709838832</v>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:26:02.926110</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>CAB:Station:69a20737-5c07-4ab4-ad8a-4fcba602ef6b</t>
+        </is>
+      </c>
+      <c r="B172" t="n">
+        <v>3</v>
+      </c>
+      <c r="C172" t="n">
+        <v>1709838832</v>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:26:02.926110</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>CAB:Station:59830a25-c7c6-4c9b-af21-0b67c836ba8f</t>
+        </is>
+      </c>
+      <c r="B173" t="n">
+        <v>5</v>
+      </c>
+      <c r="C173" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:26:02.926110</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>CAB:Station:36fe6a30-d53e-4aa8-863d-e21e80fd1d0b</t>
+        </is>
+      </c>
+      <c r="B174" t="n">
+        <v>5</v>
+      </c>
+      <c r="C174" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:26:02.926110</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>CAB:Station:ca41b63e-9046-442f-880e-d0e9186e507a</t>
+        </is>
+      </c>
+      <c r="B175" t="n">
+        <v>4</v>
+      </c>
+      <c r="C175" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:26:02.926110</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>CAB:Station:714932fd-4836-4a2a-9a19-07a6d694274c</t>
+        </is>
+      </c>
+      <c r="B176" t="n">
+        <v>2</v>
+      </c>
+      <c r="C176" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:26:02.926110</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>CAB:Station:7046d131-47fd-40bd-ba63-f52590d2ee8f</t>
+        </is>
+      </c>
+      <c r="B177" t="n">
+        <v>2</v>
+      </c>
+      <c r="C177" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:26:02.926110</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>CAB:Station:e375c577-ca9b-4f3d-b052-582f4eeeb0a8</t>
+        </is>
+      </c>
+      <c r="B178" t="n">
+        <v>3</v>
+      </c>
+      <c r="C178" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:26:02.926110</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>CAB:Station:f384359e-349d-47cf-aec3-031f20b8e0a0</t>
+        </is>
+      </c>
+      <c r="B179" t="n">
+        <v>2</v>
+      </c>
+      <c r="C179" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:26:02.926110</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>CAB:Station:e73ff873-8f43-41b4-868a-2d3e00f2cfbb</t>
+        </is>
+      </c>
+      <c r="B180" t="n">
+        <v>3</v>
+      </c>
+      <c r="C180" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:26:02.926110</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>CAB:Station:c070e40c-98f6-45d6-9543-90ceceef63af</t>
+        </is>
+      </c>
+      <c r="B181" t="n">
+        <v>8</v>
+      </c>
+      <c r="C181" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:26:02.926110</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>CAB:Station:2263b695-db35-4bbf-b70a-032920fadf3f</t>
+        </is>
+      </c>
+      <c r="B182" t="n">
+        <v>0</v>
+      </c>
+      <c r="C182" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:26:02.926110</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>CAB:Station:be796eb3-49af-494c-b3f0-dc1f0132eb7d</t>
+        </is>
+      </c>
+      <c r="B183" t="n">
+        <v>1</v>
+      </c>
+      <c r="C183" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:26:02.926110</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>CAB:Station:b207ab7a-f23d-40f8-aa26-5d02077fc6f9</t>
+        </is>
+      </c>
+      <c r="B184" t="n">
+        <v>1</v>
+      </c>
+      <c r="C184" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:26:02.926110</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>CAB:Station:958219cd-8009-45b6-8a04-1cc4ae763307</t>
+        </is>
+      </c>
+      <c r="B185" t="n">
+        <v>5</v>
+      </c>
+      <c r="C185" t="n">
+        <v>1709838832</v>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:41:03.424836</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>CAB:Station:69a20737-5c07-4ab4-ad8a-4fcba602ef6b</t>
+        </is>
+      </c>
+      <c r="B186" t="n">
+        <v>3</v>
+      </c>
+      <c r="C186" t="n">
+        <v>1709838832</v>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:41:03.424836</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>CAB:Station:59830a25-c7c6-4c9b-af21-0b67c836ba8f</t>
+        </is>
+      </c>
+      <c r="B187" t="n">
+        <v>5</v>
+      </c>
+      <c r="C187" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:41:03.424836</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>CAB:Station:36fe6a30-d53e-4aa8-863d-e21e80fd1d0b</t>
+        </is>
+      </c>
+      <c r="B188" t="n">
+        <v>5</v>
+      </c>
+      <c r="C188" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:41:03.424836</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>CAB:Station:ca41b63e-9046-442f-880e-d0e9186e507a</t>
+        </is>
+      </c>
+      <c r="B189" t="n">
+        <v>4</v>
+      </c>
+      <c r="C189" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:41:03.424836</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>CAB:Station:714932fd-4836-4a2a-9a19-07a6d694274c</t>
+        </is>
+      </c>
+      <c r="B190" t="n">
+        <v>2</v>
+      </c>
+      <c r="C190" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:41:03.424836</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>CAB:Station:7046d131-47fd-40bd-ba63-f52590d2ee8f</t>
+        </is>
+      </c>
+      <c r="B191" t="n">
+        <v>2</v>
+      </c>
+      <c r="C191" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:41:03.424836</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>CAB:Station:e375c577-ca9b-4f3d-b052-582f4eeeb0a8</t>
+        </is>
+      </c>
+      <c r="B192" t="n">
+        <v>3</v>
+      </c>
+      <c r="C192" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:41:03.424836</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>CAB:Station:f384359e-349d-47cf-aec3-031f20b8e0a0</t>
+        </is>
+      </c>
+      <c r="B193" t="n">
+        <v>2</v>
+      </c>
+      <c r="C193" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:41:03.424836</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>CAB:Station:e73ff873-8f43-41b4-868a-2d3e00f2cfbb</t>
+        </is>
+      </c>
+      <c r="B194" t="n">
+        <v>3</v>
+      </c>
+      <c r="C194" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:41:03.424836</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>CAB:Station:c070e40c-98f6-45d6-9543-90ceceef63af</t>
+        </is>
+      </c>
+      <c r="B195" t="n">
+        <v>8</v>
+      </c>
+      <c r="C195" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:41:03.424836</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>CAB:Station:2263b695-db35-4bbf-b70a-032920fadf3f</t>
+        </is>
+      </c>
+      <c r="B196" t="n">
+        <v>0</v>
+      </c>
+      <c r="C196" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:41:03.424836</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>CAB:Station:be796eb3-49af-494c-b3f0-dc1f0132eb7d</t>
+        </is>
+      </c>
+      <c r="B197" t="n">
+        <v>1</v>
+      </c>
+      <c r="C197" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:41:03.424836</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>CAB:Station:b207ab7a-f23d-40f8-aa26-5d02077fc6f9</t>
+        </is>
+      </c>
+      <c r="B198" t="n">
+        <v>1</v>
+      </c>
+      <c r="C198" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:41:03.424836</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>CAB:Station:958219cd-8009-45b6-8a04-1cc4ae763307</t>
+        </is>
+      </c>
+      <c r="B199" t="n">
+        <v>5</v>
+      </c>
+      <c r="C199" t="n">
+        <v>1709838832</v>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:56:03.906105</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>CAB:Station:69a20737-5c07-4ab4-ad8a-4fcba602ef6b</t>
+        </is>
+      </c>
+      <c r="B200" t="n">
+        <v>3</v>
+      </c>
+      <c r="C200" t="n">
+        <v>1709838832</v>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:56:03.906105</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>CAB:Station:59830a25-c7c6-4c9b-af21-0b67c836ba8f</t>
+        </is>
+      </c>
+      <c r="B201" t="n">
+        <v>5</v>
+      </c>
+      <c r="C201" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:56:03.906105</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>CAB:Station:36fe6a30-d53e-4aa8-863d-e21e80fd1d0b</t>
+        </is>
+      </c>
+      <c r="B202" t="n">
+        <v>5</v>
+      </c>
+      <c r="C202" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:56:03.906105</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>CAB:Station:ca41b63e-9046-442f-880e-d0e9186e507a</t>
+        </is>
+      </c>
+      <c r="B203" t="n">
+        <v>4</v>
+      </c>
+      <c r="C203" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:56:03.906105</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>CAB:Station:714932fd-4836-4a2a-9a19-07a6d694274c</t>
+        </is>
+      </c>
+      <c r="B204" t="n">
+        <v>2</v>
+      </c>
+      <c r="C204" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:56:03.906105</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>CAB:Station:7046d131-47fd-40bd-ba63-f52590d2ee8f</t>
+        </is>
+      </c>
+      <c r="B205" t="n">
+        <v>2</v>
+      </c>
+      <c r="C205" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:56:03.906105</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>CAB:Station:e375c577-ca9b-4f3d-b052-582f4eeeb0a8</t>
+        </is>
+      </c>
+      <c r="B206" t="n">
+        <v>3</v>
+      </c>
+      <c r="C206" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:56:03.906105</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>CAB:Station:f384359e-349d-47cf-aec3-031f20b8e0a0</t>
+        </is>
+      </c>
+      <c r="B207" t="n">
+        <v>2</v>
+      </c>
+      <c r="C207" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:56:03.906105</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>CAB:Station:e73ff873-8f43-41b4-868a-2d3e00f2cfbb</t>
+        </is>
+      </c>
+      <c r="B208" t="n">
+        <v>3</v>
+      </c>
+      <c r="C208" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:56:03.906105</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>CAB:Station:c070e40c-98f6-45d6-9543-90ceceef63af</t>
+        </is>
+      </c>
+      <c r="B209" t="n">
+        <v>8</v>
+      </c>
+      <c r="C209" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:56:03.906105</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>CAB:Station:2263b695-db35-4bbf-b70a-032920fadf3f</t>
+        </is>
+      </c>
+      <c r="B210" t="n">
+        <v>0</v>
+      </c>
+      <c r="C210" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:56:03.906105</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>CAB:Station:be796eb3-49af-494c-b3f0-dc1f0132eb7d</t>
+        </is>
+      </c>
+      <c r="B211" t="n">
+        <v>1</v>
+      </c>
+      <c r="C211" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:56:03.906105</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>CAB:Station:b207ab7a-f23d-40f8-aa26-5d02077fc6f9</t>
+        </is>
+      </c>
+      <c r="B212" t="n">
+        <v>1</v>
+      </c>
+      <c r="C212" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>2024-03-08 08:56:03.906105</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>CAB:Station:958219cd-8009-45b6-8a04-1cc4ae763307</t>
+        </is>
+      </c>
+      <c r="B213" t="n">
+        <v>5</v>
+      </c>
+      <c r="C213" t="n">
+        <v>1709838832</v>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:11:04.396364</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>CAB:Station:69a20737-5c07-4ab4-ad8a-4fcba602ef6b</t>
+        </is>
+      </c>
+      <c r="B214" t="n">
+        <v>3</v>
+      </c>
+      <c r="C214" t="n">
+        <v>1709838832</v>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:11:04.396364</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>CAB:Station:59830a25-c7c6-4c9b-af21-0b67c836ba8f</t>
+        </is>
+      </c>
+      <c r="B215" t="n">
+        <v>5</v>
+      </c>
+      <c r="C215" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:11:04.396364</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>CAB:Station:36fe6a30-d53e-4aa8-863d-e21e80fd1d0b</t>
+        </is>
+      </c>
+      <c r="B216" t="n">
+        <v>5</v>
+      </c>
+      <c r="C216" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:11:04.396364</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>CAB:Station:ca41b63e-9046-442f-880e-d0e9186e507a</t>
+        </is>
+      </c>
+      <c r="B217" t="n">
+        <v>4</v>
+      </c>
+      <c r="C217" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:11:04.396364</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>CAB:Station:714932fd-4836-4a2a-9a19-07a6d694274c</t>
+        </is>
+      </c>
+      <c r="B218" t="n">
+        <v>2</v>
+      </c>
+      <c r="C218" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:11:04.396364</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>CAB:Station:7046d131-47fd-40bd-ba63-f52590d2ee8f</t>
+        </is>
+      </c>
+      <c r="B219" t="n">
+        <v>2</v>
+      </c>
+      <c r="C219" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:11:04.396364</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>CAB:Station:e375c577-ca9b-4f3d-b052-582f4eeeb0a8</t>
+        </is>
+      </c>
+      <c r="B220" t="n">
+        <v>3</v>
+      </c>
+      <c r="C220" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:11:04.396364</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>CAB:Station:f384359e-349d-47cf-aec3-031f20b8e0a0</t>
+        </is>
+      </c>
+      <c r="B221" t="n">
+        <v>2</v>
+      </c>
+      <c r="C221" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:11:04.396364</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>CAB:Station:e73ff873-8f43-41b4-868a-2d3e00f2cfbb</t>
+        </is>
+      </c>
+      <c r="B222" t="n">
+        <v>3</v>
+      </c>
+      <c r="C222" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:11:04.396364</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>CAB:Station:c070e40c-98f6-45d6-9543-90ceceef63af</t>
+        </is>
+      </c>
+      <c r="B223" t="n">
+        <v>8</v>
+      </c>
+      <c r="C223" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:11:04.396364</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>CAB:Station:2263b695-db35-4bbf-b70a-032920fadf3f</t>
+        </is>
+      </c>
+      <c r="B224" t="n">
+        <v>0</v>
+      </c>
+      <c r="C224" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:11:04.396364</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>CAB:Station:be796eb3-49af-494c-b3f0-dc1f0132eb7d</t>
+        </is>
+      </c>
+      <c r="B225" t="n">
+        <v>1</v>
+      </c>
+      <c r="C225" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:11:04.396364</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>CAB:Station:b207ab7a-f23d-40f8-aa26-5d02077fc6f9</t>
+        </is>
+      </c>
+      <c r="B226" t="n">
+        <v>1</v>
+      </c>
+      <c r="C226" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:11:04.396364</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>CAB:Station:958219cd-8009-45b6-8a04-1cc4ae763307</t>
+        </is>
+      </c>
+      <c r="B227" t="n">
+        <v>5</v>
+      </c>
+      <c r="C227" t="n">
+        <v>1709838832</v>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:26:04.877232</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>CAB:Station:69a20737-5c07-4ab4-ad8a-4fcba602ef6b</t>
+        </is>
+      </c>
+      <c r="B228" t="n">
+        <v>3</v>
+      </c>
+      <c r="C228" t="n">
+        <v>1709838832</v>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:26:04.877232</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>CAB:Station:59830a25-c7c6-4c9b-af21-0b67c836ba8f</t>
+        </is>
+      </c>
+      <c r="B229" t="n">
+        <v>5</v>
+      </c>
+      <c r="C229" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:26:04.877232</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>CAB:Station:36fe6a30-d53e-4aa8-863d-e21e80fd1d0b</t>
+        </is>
+      </c>
+      <c r="B230" t="n">
+        <v>5</v>
+      </c>
+      <c r="C230" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:26:04.877232</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>CAB:Station:ca41b63e-9046-442f-880e-d0e9186e507a</t>
+        </is>
+      </c>
+      <c r="B231" t="n">
+        <v>4</v>
+      </c>
+      <c r="C231" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:26:04.877232</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>CAB:Station:714932fd-4836-4a2a-9a19-07a6d694274c</t>
+        </is>
+      </c>
+      <c r="B232" t="n">
+        <v>2</v>
+      </c>
+      <c r="C232" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:26:04.877232</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>CAB:Station:7046d131-47fd-40bd-ba63-f52590d2ee8f</t>
+        </is>
+      </c>
+      <c r="B233" t="n">
+        <v>2</v>
+      </c>
+      <c r="C233" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:26:04.877232</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>CAB:Station:e375c577-ca9b-4f3d-b052-582f4eeeb0a8</t>
+        </is>
+      </c>
+      <c r="B234" t="n">
+        <v>3</v>
+      </c>
+      <c r="C234" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:26:04.877232</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>CAB:Station:f384359e-349d-47cf-aec3-031f20b8e0a0</t>
+        </is>
+      </c>
+      <c r="B235" t="n">
+        <v>2</v>
+      </c>
+      <c r="C235" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:26:04.877232</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>CAB:Station:e73ff873-8f43-41b4-868a-2d3e00f2cfbb</t>
+        </is>
+      </c>
+      <c r="B236" t="n">
+        <v>3</v>
+      </c>
+      <c r="C236" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:26:04.877232</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>CAB:Station:c070e40c-98f6-45d6-9543-90ceceef63af</t>
+        </is>
+      </c>
+      <c r="B237" t="n">
+        <v>8</v>
+      </c>
+      <c r="C237" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:26:04.877232</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>CAB:Station:2263b695-db35-4bbf-b70a-032920fadf3f</t>
+        </is>
+      </c>
+      <c r="B238" t="n">
+        <v>0</v>
+      </c>
+      <c r="C238" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:26:04.877232</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>CAB:Station:be796eb3-49af-494c-b3f0-dc1f0132eb7d</t>
+        </is>
+      </c>
+      <c r="B239" t="n">
+        <v>1</v>
+      </c>
+      <c r="C239" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:26:04.877232</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>CAB:Station:b207ab7a-f23d-40f8-aa26-5d02077fc6f9</t>
+        </is>
+      </c>
+      <c r="B240" t="n">
+        <v>1</v>
+      </c>
+      <c r="C240" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:26:04.877232</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>CAB:Station:958219cd-8009-45b6-8a04-1cc4ae763307</t>
+        </is>
+      </c>
+      <c r="B241" t="n">
+        <v>5</v>
+      </c>
+      <c r="C241" t="n">
+        <v>1709838832</v>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:41:05.420553</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>CAB:Station:69a20737-5c07-4ab4-ad8a-4fcba602ef6b</t>
+        </is>
+      </c>
+      <c r="B242" t="n">
+        <v>3</v>
+      </c>
+      <c r="C242" t="n">
+        <v>1709838832</v>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:41:05.420553</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>CAB:Station:59830a25-c7c6-4c9b-af21-0b67c836ba8f</t>
+        </is>
+      </c>
+      <c r="B243" t="n">
+        <v>5</v>
+      </c>
+      <c r="C243" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:41:05.420553</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>CAB:Station:36fe6a30-d53e-4aa8-863d-e21e80fd1d0b</t>
+        </is>
+      </c>
+      <c r="B244" t="n">
+        <v>5</v>
+      </c>
+      <c r="C244" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:41:05.420553</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>CAB:Station:ca41b63e-9046-442f-880e-d0e9186e507a</t>
+        </is>
+      </c>
+      <c r="B245" t="n">
+        <v>4</v>
+      </c>
+      <c r="C245" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:41:05.420553</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>CAB:Station:714932fd-4836-4a2a-9a19-07a6d694274c</t>
+        </is>
+      </c>
+      <c r="B246" t="n">
+        <v>2</v>
+      </c>
+      <c r="C246" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:41:05.420553</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>CAB:Station:7046d131-47fd-40bd-ba63-f52590d2ee8f</t>
+        </is>
+      </c>
+      <c r="B247" t="n">
+        <v>2</v>
+      </c>
+      <c r="C247" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:41:05.420553</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>CAB:Station:e375c577-ca9b-4f3d-b052-582f4eeeb0a8</t>
+        </is>
+      </c>
+      <c r="B248" t="n">
+        <v>3</v>
+      </c>
+      <c r="C248" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:41:05.420553</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>CAB:Station:f384359e-349d-47cf-aec3-031f20b8e0a0</t>
+        </is>
+      </c>
+      <c r="B249" t="n">
+        <v>2</v>
+      </c>
+      <c r="C249" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:41:05.420553</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>CAB:Station:e73ff873-8f43-41b4-868a-2d3e00f2cfbb</t>
+        </is>
+      </c>
+      <c r="B250" t="n">
+        <v>3</v>
+      </c>
+      <c r="C250" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:41:05.420553</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>CAB:Station:c070e40c-98f6-45d6-9543-90ceceef63af</t>
+        </is>
+      </c>
+      <c r="B251" t="n">
+        <v>8</v>
+      </c>
+      <c r="C251" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:41:05.420553</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>CAB:Station:2263b695-db35-4bbf-b70a-032920fadf3f</t>
+        </is>
+      </c>
+      <c r="B252" t="n">
+        <v>0</v>
+      </c>
+      <c r="C252" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:41:05.420553</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>CAB:Station:be796eb3-49af-494c-b3f0-dc1f0132eb7d</t>
+        </is>
+      </c>
+      <c r="B253" t="n">
+        <v>1</v>
+      </c>
+      <c r="C253" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:41:05.420553</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>CAB:Station:b207ab7a-f23d-40f8-aa26-5d02077fc6f9</t>
+        </is>
+      </c>
+      <c r="B254" t="n">
+        <v>1</v>
+      </c>
+      <c r="C254" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:41:05.420553</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>CAB:Station:958219cd-8009-45b6-8a04-1cc4ae763307</t>
+        </is>
+      </c>
+      <c r="B255" t="n">
+        <v>5</v>
+      </c>
+      <c r="C255" t="n">
+        <v>1709838832</v>
+      </c>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:56:05.907785</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>CAB:Station:69a20737-5c07-4ab4-ad8a-4fcba602ef6b</t>
+        </is>
+      </c>
+      <c r="B256" t="n">
+        <v>3</v>
+      </c>
+      <c r="C256" t="n">
+        <v>1709838832</v>
+      </c>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:56:05.907785</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>CAB:Station:59830a25-c7c6-4c9b-af21-0b67c836ba8f</t>
+        </is>
+      </c>
+      <c r="B257" t="n">
+        <v>5</v>
+      </c>
+      <c r="C257" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:56:05.907785</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>CAB:Station:36fe6a30-d53e-4aa8-863d-e21e80fd1d0b</t>
+        </is>
+      </c>
+      <c r="B258" t="n">
+        <v>5</v>
+      </c>
+      <c r="C258" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:56:05.907785</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>CAB:Station:ca41b63e-9046-442f-880e-d0e9186e507a</t>
+        </is>
+      </c>
+      <c r="B259" t="n">
+        <v>4</v>
+      </c>
+      <c r="C259" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:56:05.907785</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>CAB:Station:714932fd-4836-4a2a-9a19-07a6d694274c</t>
+        </is>
+      </c>
+      <c r="B260" t="n">
+        <v>2</v>
+      </c>
+      <c r="C260" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:56:05.907785</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>CAB:Station:7046d131-47fd-40bd-ba63-f52590d2ee8f</t>
+        </is>
+      </c>
+      <c r="B261" t="n">
+        <v>2</v>
+      </c>
+      <c r="C261" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:56:05.907785</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>CAB:Station:e375c577-ca9b-4f3d-b052-582f4eeeb0a8</t>
+        </is>
+      </c>
+      <c r="B262" t="n">
+        <v>3</v>
+      </c>
+      <c r="C262" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:56:05.907785</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>CAB:Station:f384359e-349d-47cf-aec3-031f20b8e0a0</t>
+        </is>
+      </c>
+      <c r="B263" t="n">
+        <v>2</v>
+      </c>
+      <c r="C263" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:56:05.907785</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>CAB:Station:e73ff873-8f43-41b4-868a-2d3e00f2cfbb</t>
+        </is>
+      </c>
+      <c r="B264" t="n">
+        <v>3</v>
+      </c>
+      <c r="C264" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:56:05.907785</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>CAB:Station:c070e40c-98f6-45d6-9543-90ceceef63af</t>
+        </is>
+      </c>
+      <c r="B265" t="n">
+        <v>8</v>
+      </c>
+      <c r="C265" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:56:05.907785</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>CAB:Station:2263b695-db35-4bbf-b70a-032920fadf3f</t>
+        </is>
+      </c>
+      <c r="B266" t="n">
+        <v>0</v>
+      </c>
+      <c r="C266" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:56:05.907785</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>CAB:Station:be796eb3-49af-494c-b3f0-dc1f0132eb7d</t>
+        </is>
+      </c>
+      <c r="B267" t="n">
+        <v>1</v>
+      </c>
+      <c r="C267" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:56:05.907785</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>CAB:Station:b207ab7a-f23d-40f8-aa26-5d02077fc6f9</t>
+        </is>
+      </c>
+      <c r="B268" t="n">
+        <v>1</v>
+      </c>
+      <c r="C268" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>2024-03-08 09:56:05.907785</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>CAB:Station:958219cd-8009-45b6-8a04-1cc4ae763307</t>
+        </is>
+      </c>
+      <c r="B269" t="n">
+        <v>5</v>
+      </c>
+      <c r="C269" t="n">
+        <v>1709838832</v>
+      </c>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>2024-03-08 10:11:06.392049</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>CAB:Station:69a20737-5c07-4ab4-ad8a-4fcba602ef6b</t>
+        </is>
+      </c>
+      <c r="B270" t="n">
+        <v>3</v>
+      </c>
+      <c r="C270" t="n">
+        <v>1709838832</v>
+      </c>
+      <c r="D270" t="inlineStr">
+        <is>
+          <t>2024-03-08 10:11:06.392049</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>CAB:Station:59830a25-c7c6-4c9b-af21-0b67c836ba8f</t>
+        </is>
+      </c>
+      <c r="B271" t="n">
+        <v>5</v>
+      </c>
+      <c r="C271" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D271" t="inlineStr">
+        <is>
+          <t>2024-03-08 10:11:06.392049</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>CAB:Station:36fe6a30-d53e-4aa8-863d-e21e80fd1d0b</t>
+        </is>
+      </c>
+      <c r="B272" t="n">
+        <v>5</v>
+      </c>
+      <c r="C272" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D272" t="inlineStr">
+        <is>
+          <t>2024-03-08 10:11:06.392049</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>CAB:Station:ca41b63e-9046-442f-880e-d0e9186e507a</t>
+        </is>
+      </c>
+      <c r="B273" t="n">
+        <v>4</v>
+      </c>
+      <c r="C273" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>2024-03-08 10:11:06.392049</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>CAB:Station:714932fd-4836-4a2a-9a19-07a6d694274c</t>
+        </is>
+      </c>
+      <c r="B274" t="n">
+        <v>2</v>
+      </c>
+      <c r="C274" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>2024-03-08 10:11:06.392049</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>CAB:Station:7046d131-47fd-40bd-ba63-f52590d2ee8f</t>
+        </is>
+      </c>
+      <c r="B275" t="n">
+        <v>2</v>
+      </c>
+      <c r="C275" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>2024-03-08 10:11:06.392049</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>CAB:Station:e375c577-ca9b-4f3d-b052-582f4eeeb0a8</t>
+        </is>
+      </c>
+      <c r="B276" t="n">
+        <v>3</v>
+      </c>
+      <c r="C276" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>2024-03-08 10:11:06.392049</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>CAB:Station:f384359e-349d-47cf-aec3-031f20b8e0a0</t>
+        </is>
+      </c>
+      <c r="B277" t="n">
+        <v>2</v>
+      </c>
+      <c r="C277" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>2024-03-08 10:11:06.392049</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>CAB:Station:e73ff873-8f43-41b4-868a-2d3e00f2cfbb</t>
+        </is>
+      </c>
+      <c r="B278" t="n">
+        <v>3</v>
+      </c>
+      <c r="C278" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>2024-03-08 10:11:06.392049</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>CAB:Station:c070e40c-98f6-45d6-9543-90ceceef63af</t>
+        </is>
+      </c>
+      <c r="B279" t="n">
+        <v>8</v>
+      </c>
+      <c r="C279" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>2024-03-08 10:11:06.392049</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>CAB:Station:2263b695-db35-4bbf-b70a-032920fadf3f</t>
+        </is>
+      </c>
+      <c r="B280" t="n">
+        <v>0</v>
+      </c>
+      <c r="C280" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>2024-03-08 10:11:06.392049</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>CAB:Station:be796eb3-49af-494c-b3f0-dc1f0132eb7d</t>
+        </is>
+      </c>
+      <c r="B281" t="n">
+        <v>1</v>
+      </c>
+      <c r="C281" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>2024-03-08 10:11:06.392049</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>CAB:Station:b207ab7a-f23d-40f8-aa26-5d02077fc6f9</t>
+        </is>
+      </c>
+      <c r="B282" t="n">
+        <v>1</v>
+      </c>
+      <c r="C282" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>2024-03-08 10:11:06.392049</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>CAB:Station:958219cd-8009-45b6-8a04-1cc4ae763307</t>
+        </is>
+      </c>
+      <c r="B283" t="n">
+        <v>5</v>
+      </c>
+      <c r="C283" t="n">
+        <v>1709838832</v>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>2024-03-08 11:11:42.393357</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>CAB:Station:69a20737-5c07-4ab4-ad8a-4fcba602ef6b</t>
+        </is>
+      </c>
+      <c r="B284" t="n">
+        <v>3</v>
+      </c>
+      <c r="C284" t="n">
+        <v>1709838832</v>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>2024-03-08 11:11:42.393357</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>CAB:Station:59830a25-c7c6-4c9b-af21-0b67c836ba8f</t>
+        </is>
+      </c>
+      <c r="B285" t="n">
+        <v>5</v>
+      </c>
+      <c r="C285" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>2024-03-08 11:11:42.393357</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>CAB:Station:36fe6a30-d53e-4aa8-863d-e21e80fd1d0b</t>
+        </is>
+      </c>
+      <c r="B286" t="n">
+        <v>5</v>
+      </c>
+      <c r="C286" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>2024-03-08 11:11:42.393357</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>CAB:Station:ca41b63e-9046-442f-880e-d0e9186e507a</t>
+        </is>
+      </c>
+      <c r="B287" t="n">
+        <v>4</v>
+      </c>
+      <c r="C287" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>2024-03-08 11:11:42.393357</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>CAB:Station:714932fd-4836-4a2a-9a19-07a6d694274c</t>
+        </is>
+      </c>
+      <c r="B288" t="n">
+        <v>2</v>
+      </c>
+      <c r="C288" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>2024-03-08 11:11:42.393357</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>CAB:Station:7046d131-47fd-40bd-ba63-f52590d2ee8f</t>
+        </is>
+      </c>
+      <c r="B289" t="n">
+        <v>2</v>
+      </c>
+      <c r="C289" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>2024-03-08 11:11:42.393357</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>CAB:Station:e375c577-ca9b-4f3d-b052-582f4eeeb0a8</t>
+        </is>
+      </c>
+      <c r="B290" t="n">
+        <v>3</v>
+      </c>
+      <c r="C290" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>2024-03-08 11:11:42.393357</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>CAB:Station:f384359e-349d-47cf-aec3-031f20b8e0a0</t>
+        </is>
+      </c>
+      <c r="B291" t="n">
+        <v>2</v>
+      </c>
+      <c r="C291" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>2024-03-08 11:11:42.393357</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>CAB:Station:e73ff873-8f43-41b4-868a-2d3e00f2cfbb</t>
+        </is>
+      </c>
+      <c r="B292" t="n">
+        <v>3</v>
+      </c>
+      <c r="C292" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>2024-03-08 11:11:42.393357</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>CAB:Station:c070e40c-98f6-45d6-9543-90ceceef63af</t>
+        </is>
+      </c>
+      <c r="B293" t="n">
+        <v>8</v>
+      </c>
+      <c r="C293" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>2024-03-08 11:11:42.393357</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>CAB:Station:2263b695-db35-4bbf-b70a-032920fadf3f</t>
+        </is>
+      </c>
+      <c r="B294" t="n">
+        <v>0</v>
+      </c>
+      <c r="C294" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>2024-03-08 11:11:42.393357</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>CAB:Station:be796eb3-49af-494c-b3f0-dc1f0132eb7d</t>
+        </is>
+      </c>
+      <c r="B295" t="n">
+        <v>1</v>
+      </c>
+      <c r="C295" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>2024-03-08 11:11:42.393357</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>CAB:Station:b207ab7a-f23d-40f8-aa26-5d02077fc6f9</t>
+        </is>
+      </c>
+      <c r="B296" t="n">
+        <v>1</v>
+      </c>
+      <c r="C296" t="n">
+        <v>1709838833</v>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>2024-03-08 11:11:42.393357</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>